<commit_message>
updates to raw data and Stata codes
</commit_message>
<xml_diff>
--- a/analytics/modified_data/tbf_crop_codes_2023.xlsx
+++ b/analytics/modified_data/tbf_crop_codes_2023.xlsx
@@ -33,6 +33,9 @@
     <t>cilantro</t>
   </si>
   <si>
+    <t>corn- ornamental, glass gem</t>
+  </si>
+  <si>
     <t>dill- hera</t>
   </si>
   <si>
@@ -51,22 +54,22 @@
     <t>pepper- anaheim</t>
   </si>
   <si>
+    <t>pepper- califonia wonder</t>
+  </si>
+  <si>
     <t xml:space="preserve">pepper- ghost </t>
   </si>
   <si>
     <t>pepper- habanero</t>
   </si>
   <si>
-    <t>pepper- jalapeno- early</t>
+    <t>pepper- jalapeno, early</t>
   </si>
   <si>
     <t>pepper- sweet banana</t>
   </si>
   <si>
-    <t>pepper- sweet- ca wonder</t>
-  </si>
-  <si>
-    <t>pumpkin- ct field</t>
+    <t>pumpkin- connecticut field</t>
   </si>
   <si>
     <t>sage- broad leaf</t>
@@ -76,9 +79,6 @@
   </si>
   <si>
     <t>sweet corn- country gentleman</t>
-  </si>
-  <si>
-    <t>sweet corn- ornamental- glas gm</t>
   </si>
   <si>
     <t>tomato- amish</t>

</xml_diff>